<commit_message>
Erica fixes dates again
</commit_message>
<xml_diff>
--- a/data/source_pops/source_pop_Kluane_shrub_data/weekly_subsets/160722_EZ_weekly_source_pop_Kluane_2022.xlsx
+++ b/data/source_pops/source_pop_Kluane_shrub_data/weekly_subsets/160722_EZ_weekly_source_pop_Kluane_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazaja/Desktop/MRes/MSc_ZAJA_2022/data/source_pop_Kluane_shrub_data/weekly_subsets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazaja/Desktop/Github_repos.tmp/GardenHub/data/source_pops/source_pop_Kluane_shrub_data/weekly_subsets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A667AEA2-3171-224E-A222-1D9F70F2E2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30688267-314D-9F4E-ACF0-CA87DB376697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7980" yWindow="540" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -241,6 +241,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -389,8 +395,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="33">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -416,24 +422,16 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -455,7 +453,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -469,6 +466,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,13 +688,13 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q1" sqref="Q1"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="31" customWidth="1"/>
-    <col min="2" max="5" width="10.5" style="31" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="5" width="10.5" customWidth="1"/>
     <col min="6" max="7" width="16.6640625" customWidth="1"/>
     <col min="8" max="19" width="10.5" customWidth="1"/>
     <col min="20" max="21" width="60.83203125" customWidth="1"/>
@@ -722,43 +720,43 @@
       <c r="F1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="N1" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="O1" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="28" t="s">
         <v>47</v>
       </c>
       <c r="Q1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="R1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="S1" s="28" t="s">
         <v>49</v>
       </c>
       <c r="T1" s="2" t="s">
@@ -786,56 +784,56 @@
       <c r="A2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="21">
         <v>60.970199999999998</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="21">
         <v>138.41289</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="21">
         <v>1580</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F2" s="32">
         <v>44758</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="18">
+      <c r="H2" s="11">
         <v>195</v>
       </c>
-      <c r="I2" s="18">
+      <c r="I2" s="11">
         <v>285</v>
       </c>
-      <c r="J2" s="18">
+      <c r="J2" s="11">
         <v>168</v>
       </c>
-      <c r="K2" s="18">
+      <c r="K2" s="11">
         <v>47</v>
       </c>
-      <c r="L2" s="18">
+      <c r="L2" s="11">
         <v>23</v>
       </c>
-      <c r="M2" s="18">
+      <c r="M2" s="11">
         <v>44</v>
       </c>
-      <c r="N2" s="18">
+      <c r="N2" s="11">
         <v>74</v>
       </c>
-      <c r="O2" s="18">
+      <c r="O2" s="11">
         <v>54</v>
       </c>
-      <c r="P2" s="18">
+      <c r="P2" s="11">
         <v>57</v>
       </c>
-      <c r="Q2" s="18">
+      <c r="Q2" s="11">
         <v>122</v>
       </c>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
       <c r="V2" s="1"/>
@@ -859,58 +857,58 @@
       <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="21">
         <v>60.970100000000002</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="21">
         <v>138.4128</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="21">
         <v>1581</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="32">
         <v>44758</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="11">
         <v>152</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="11">
         <v>118</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="11">
         <v>98</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="11">
         <v>132</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="11">
         <v>111</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="11">
         <v>124</v>
       </c>
-      <c r="N3" s="18">
+      <c r="N3" s="11">
         <v>77</v>
       </c>
-      <c r="O3" s="18">
+      <c r="O3" s="11">
         <v>70</v>
       </c>
-      <c r="P3" s="18">
+      <c r="P3" s="11">
         <v>55</v>
       </c>
-      <c r="Q3" s="18">
+      <c r="Q3" s="11">
         <v>43</v>
       </c>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -932,56 +930,56 @@
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="21">
         <v>60.970080000000003</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="21">
         <v>138.4127</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="21">
         <v>1582</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="32">
         <v>44758</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="11">
         <v>155</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="11">
         <v>125</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="11">
         <v>220</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="11">
         <v>66</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="11">
         <v>104</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="11">
         <v>160</v>
       </c>
-      <c r="N4" s="18">
+      <c r="N4" s="11">
         <v>50</v>
       </c>
-      <c r="O4" s="18">
+      <c r="O4" s="11">
         <v>48</v>
       </c>
-      <c r="P4" s="18">
+      <c r="P4" s="11">
         <v>46</v>
       </c>
-      <c r="Q4" s="18">
+      <c r="Q4" s="11">
         <v>41</v>
       </c>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
       <c r="T4" s="13"/>
       <c r="U4" s="13"/>
       <c r="V4" s="1"/>
@@ -1005,56 +1003,56 @@
       <c r="A5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="21">
         <v>60.970149999999997</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="21">
         <v>138.41316</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="21">
         <v>1580</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="32">
         <v>44758</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="11">
         <v>174</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="11">
         <v>179</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="11">
         <v>130</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="11">
         <v>86</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="11">
         <v>106</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="11">
         <v>85</v>
       </c>
-      <c r="N5" s="18">
+      <c r="N5" s="11">
         <v>58</v>
       </c>
-      <c r="O5" s="18">
+      <c r="O5" s="11">
         <v>62</v>
       </c>
-      <c r="P5" s="18">
+      <c r="P5" s="11">
         <v>45</v>
       </c>
-      <c r="Q5" s="18">
+      <c r="Q5" s="11">
         <v>46</v>
       </c>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
       <c r="T5" s="10"/>
       <c r="U5" s="13"/>
       <c r="V5" s="1"/>
@@ -1078,56 +1076,56 @@
       <c r="A6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="21">
         <v>60.969880000000003</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="21">
         <v>138.41269</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="21">
         <v>1583</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="32">
         <v>44758</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="11">
         <v>176</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="11">
         <v>286</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="11">
         <v>255</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="11">
         <v>102</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="11">
         <v>76</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="11">
         <v>107</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="11">
         <v>58</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="11">
         <v>53</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="11">
         <v>65</v>
       </c>
-      <c r="Q6" s="18">
+      <c r="Q6" s="11">
         <v>48</v>
       </c>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
@@ -1149,58 +1147,58 @@
       <c r="A7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="21">
         <v>60.971850000000003</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="21">
         <v>138.41123999999999</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="21">
         <v>1552</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="32">
         <v>44758</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="11">
         <v>177</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="11">
         <v>153</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="11">
         <v>190</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="11">
         <v>95</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="11">
         <v>70</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="11">
         <v>77</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="11">
         <v>63</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="11">
         <v>47</v>
       </c>
-      <c r="P7" s="18">
+      <c r="P7" s="11">
         <v>63</v>
       </c>
-      <c r="Q7" s="18">
+      <c r="Q7" s="11">
         <v>52</v>
       </c>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="14"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="13"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
@@ -1222,58 +1220,58 @@
       <c r="A8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="21">
         <v>60.972059999999999</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="21">
         <v>138.41098</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="21">
         <v>1549</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="32">
         <v>44758</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="11">
         <v>83</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="11">
         <v>99</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="11">
         <v>123</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="11">
         <v>33</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="11">
         <v>105</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="11">
         <v>104</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="11">
         <v>55</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="11">
         <v>62</v>
       </c>
-      <c r="P8" s="18">
+      <c r="P8" s="11">
         <v>55</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="Q8" s="11">
         <v>20</v>
       </c>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="14"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="13"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
@@ -1295,58 +1293,58 @@
       <c r="A9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="21">
         <v>60.971989999999998</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="21">
         <v>138.41195999999999</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="21">
         <v>1547</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="32">
         <v>44758</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="11">
         <v>123</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="11">
         <v>167</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="11">
         <v>175</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="11">
         <v>50</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="11">
         <v>28</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="11">
         <v>57</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="11">
         <v>51</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O9" s="11">
         <v>40</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="11">
         <v>43</v>
       </c>
-      <c r="Q9" s="18">
+      <c r="Q9" s="11">
         <v>34</v>
       </c>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="14"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="13"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
@@ -1368,58 +1366,58 @@
       <c r="A10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="21">
         <v>60.972000000000001</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="21">
         <v>138.41204999999999</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="21">
         <v>1548</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="32">
         <v>44758</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="11">
         <v>157</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="11">
         <v>203</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="11">
         <v>145</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="11">
         <v>55</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="11">
         <v>124</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="11">
         <v>141</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="11">
         <v>68</v>
       </c>
-      <c r="O10" s="18">
+      <c r="O10" s="11">
         <v>62</v>
       </c>
-      <c r="P10" s="18">
+      <c r="P10" s="11">
         <v>67</v>
       </c>
-      <c r="Q10" s="18">
+      <c r="Q10" s="11">
         <v>56</v>
       </c>
-      <c r="R10" s="27"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="14"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="13"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
@@ -1441,58 +1439,58 @@
       <c r="A11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="21">
         <v>60.971530000000001</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="21">
         <v>138.41092</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="21">
         <v>1553</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="32">
         <v>44758</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="11">
         <v>66</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="11">
         <v>96</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="11">
         <v>107</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="11">
         <v>34</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="11">
         <v>35</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="11">
         <v>19</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="11">
         <v>49</v>
       </c>
-      <c r="O11" s="18">
+      <c r="O11" s="11">
         <v>60</v>
       </c>
-      <c r="P11" s="18">
+      <c r="P11" s="11">
         <v>48</v>
       </c>
-      <c r="Q11" s="18">
+      <c r="Q11" s="11">
         <v>16</v>
       </c>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="14"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="13"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
@@ -1511,61 +1509,61 @@
       <c r="AK11" s="1"/>
     </row>
     <row r="12" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="21">
         <v>60.970149999999997</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="21">
         <v>138.41283000000001</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="21">
         <v>1581</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="32">
         <v>44758</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="11">
         <v>143</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="11">
         <v>154</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="11">
         <v>109</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="11">
         <v>46</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="11">
         <v>54</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="11">
         <v>86</v>
       </c>
-      <c r="N12" s="18">
+      <c r="N12" s="11">
         <v>44</v>
       </c>
-      <c r="O12" s="18">
+      <c r="O12" s="11">
         <v>55</v>
       </c>
-      <c r="P12" s="18">
+      <c r="P12" s="11">
         <v>48</v>
       </c>
-      <c r="Q12" s="18">
+      <c r="Q12" s="11">
         <v>52</v>
       </c>
-      <c r="R12" s="27"/>
-      <c r="S12" s="27"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="14"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="13"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
@@ -1584,59 +1582,59 @@
       <c r="AK12" s="1"/>
     </row>
     <row r="13" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="21">
         <v>60.970100000000002</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="21">
         <v>138.41283000000001</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="21">
         <v>1581</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="32">
         <v>44758</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="11">
         <v>125.5</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="11">
         <v>110</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="11">
         <v>164</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="11">
         <v>51</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="11">
         <v>82</v>
       </c>
-      <c r="M13" s="21">
+      <c r="M13" s="17">
         <v>75</v>
       </c>
-      <c r="N13" s="18">
+      <c r="N13" s="11">
         <v>38</v>
       </c>
-      <c r="O13" s="18">
+      <c r="O13" s="11">
         <v>61</v>
       </c>
-      <c r="P13" s="18">
+      <c r="P13" s="11">
         <v>49</v>
       </c>
-      <c r="Q13" s="18">
+      <c r="Q13" s="11">
         <v>40</v>
       </c>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
       <c r="T13" s="11"/>
       <c r="U13" s="12"/>
       <c r="V13" s="1"/>
@@ -1657,61 +1655,61 @@
       <c r="AK13" s="1"/>
     </row>
     <row r="14" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="21">
         <v>60.970120000000001</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="21">
         <v>138.41273000000001</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="21">
         <v>1581</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="32">
         <v>44758</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="11">
         <v>145</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="11">
         <v>200</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="11">
         <v>154</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14" s="11">
         <v>75</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="11">
         <v>60</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="11">
         <v>46</v>
       </c>
-      <c r="N14" s="18">
+      <c r="N14" s="11">
         <v>53</v>
       </c>
-      <c r="O14" s="18">
+      <c r="O14" s="11">
         <v>45</v>
       </c>
-      <c r="P14" s="18">
+      <c r="P14" s="11">
         <v>53</v>
       </c>
-      <c r="Q14" s="18">
+      <c r="Q14" s="11">
         <v>65</v>
       </c>
-      <c r="R14" s="29"/>
-      <c r="S14" s="29"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
@@ -1730,61 +1728,61 @@
       <c r="AK14" s="1"/>
     </row>
     <row r="15" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="21">
         <v>60.970050000000001</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="21">
         <v>138.41264000000001</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="21">
         <v>1582</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="32">
         <v>44758</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="11">
         <v>140</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="11">
         <v>139</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="11">
         <v>144</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="11">
         <v>108</v>
       </c>
-      <c r="L15" s="18">
+      <c r="L15" s="11">
         <v>160</v>
       </c>
-      <c r="M15" s="18">
+      <c r="M15" s="11">
         <v>155</v>
       </c>
-      <c r="N15" s="18">
+      <c r="N15" s="11">
         <v>43</v>
       </c>
-      <c r="O15" s="18">
+      <c r="O15" s="11">
         <v>41</v>
       </c>
-      <c r="P15" s="18">
+      <c r="P15" s="11">
         <v>38</v>
       </c>
-      <c r="Q15" s="17">
+      <c r="Q15" s="12">
         <v>57</v>
       </c>
-      <c r="R15" s="29"/>
-      <c r="S15" s="29"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="17"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="12"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
@@ -1803,61 +1801,61 @@
       <c r="AK15" s="1"/>
     </row>
     <row r="16" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="21">
         <v>60.970050000000001</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="21">
         <v>138.41322</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="21">
         <v>1582</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="32">
         <v>44758</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="11">
         <v>155.19999999999999</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="11">
         <v>171</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="11">
         <v>184</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K16" s="11">
         <v>80</v>
       </c>
-      <c r="L16" s="18">
+      <c r="L16" s="11">
         <v>137</v>
       </c>
-      <c r="M16" s="18">
+      <c r="M16" s="11">
         <v>170</v>
       </c>
-      <c r="N16" s="18">
+      <c r="N16" s="11">
         <v>55</v>
       </c>
-      <c r="O16" s="18">
+      <c r="O16" s="11">
         <v>50</v>
       </c>
-      <c r="P16" s="18">
+      <c r="P16" s="11">
         <v>48</v>
       </c>
-      <c r="Q16" s="18">
+      <c r="Q16" s="11">
         <v>46</v>
       </c>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="17"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="12"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
@@ -1876,61 +1874,61 @@
       <c r="AK16" s="1"/>
     </row>
     <row r="17" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="21">
         <v>60.971980000000002</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="21">
         <v>138.41140999999999</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="21">
         <v>1550</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="32">
         <v>44758</v>
       </c>
-      <c r="G17" s="30" t="s">
+      <c r="G17" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="11">
         <v>132</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="11">
         <v>236</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="11">
         <v>242</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="11">
         <v>120</v>
       </c>
-      <c r="L17" s="18">
+      <c r="L17" s="11">
         <v>138</v>
       </c>
-      <c r="M17" s="18">
+      <c r="M17" s="11">
         <v>160</v>
       </c>
-      <c r="N17" s="18">
+      <c r="N17" s="11">
         <v>51</v>
       </c>
-      <c r="O17" s="18">
+      <c r="O17" s="11">
         <v>56</v>
       </c>
-      <c r="P17" s="18">
+      <c r="P17" s="11">
         <v>38</v>
       </c>
-      <c r="Q17" s="18">
+      <c r="Q17" s="11">
         <v>67</v>
       </c>
-      <c r="R17" s="27"/>
-      <c r="S17" s="27"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="17"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="12"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
@@ -1949,61 +1947,61 @@
       <c r="AK17" s="1"/>
     </row>
     <row r="18" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="21">
         <v>60.971989999999998</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="21">
         <v>138.41204999999999</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="21">
         <v>1547</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="32">
         <v>44758</v>
       </c>
-      <c r="G18" s="30" t="s">
+      <c r="G18" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="11">
         <v>159</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="11">
         <v>163</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="11">
         <v>173</v>
       </c>
-      <c r="K18" s="18">
+      <c r="K18" s="11">
         <v>141</v>
       </c>
-      <c r="L18" s="18">
+      <c r="L18" s="11">
         <v>124</v>
       </c>
-      <c r="M18" s="18">
+      <c r="M18" s="11">
         <v>75</v>
       </c>
-      <c r="N18" s="18">
+      <c r="N18" s="11">
         <v>43</v>
       </c>
-      <c r="O18" s="18">
+      <c r="O18" s="11">
         <v>53</v>
       </c>
-      <c r="P18" s="18">
+      <c r="P18" s="11">
         <v>55</v>
       </c>
-      <c r="Q18" s="18">
+      <c r="Q18" s="11">
         <v>46</v>
       </c>
-      <c r="R18" s="27"/>
-      <c r="S18" s="27"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="17"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="12"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
@@ -2022,61 +2020,61 @@
       <c r="AK18" s="1"/>
     </row>
     <row r="19" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="21">
         <v>60.97193</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="21">
         <v>138.41200000000001</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="21">
         <v>1550</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="32">
         <v>44758</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="11">
         <v>171</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="11">
         <v>245</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="11">
         <v>221</v>
       </c>
-      <c r="K19" s="18">
+      <c r="K19" s="11">
         <v>80</v>
       </c>
-      <c r="L19" s="18">
+      <c r="L19" s="11">
         <v>45</v>
       </c>
-      <c r="M19" s="18">
+      <c r="M19" s="11">
         <v>100</v>
       </c>
-      <c r="N19" s="18">
+      <c r="N19" s="11">
         <v>45</v>
       </c>
-      <c r="O19" s="18">
+      <c r="O19" s="11">
         <v>48</v>
       </c>
-      <c r="P19" s="18">
+      <c r="P19" s="11">
         <v>58</v>
       </c>
-      <c r="Q19" s="18">
+      <c r="Q19" s="11">
         <v>46</v>
       </c>
-      <c r="R19" s="27"/>
-      <c r="S19" s="27"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="17"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="12"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
@@ -2095,61 +2093,61 @@
       <c r="AK19" s="1"/>
     </row>
     <row r="20" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="21">
         <v>60.97213</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="21">
         <v>138.41197</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="21">
         <v>1546</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="32">
         <v>44758</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G20" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H20" s="11">
         <v>84.5</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="11">
         <v>81</v>
       </c>
-      <c r="J20" s="18">
+      <c r="J20" s="11">
         <v>73</v>
       </c>
-      <c r="K20" s="18">
+      <c r="K20" s="11">
         <v>37</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="11">
         <v>47</v>
       </c>
-      <c r="M20" s="18">
+      <c r="M20" s="11">
         <v>31</v>
       </c>
-      <c r="N20" s="18">
+      <c r="N20" s="11">
         <v>42</v>
       </c>
-      <c r="O20" s="18">
+      <c r="O20" s="11">
         <v>44</v>
       </c>
-      <c r="P20" s="18">
+      <c r="P20" s="11">
         <v>37</v>
       </c>
-      <c r="Q20" s="18">
+      <c r="Q20" s="11">
         <v>24</v>
       </c>
-      <c r="R20" s="27"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="18"/>
-      <c r="U20" s="17"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="12"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
@@ -2168,61 +2166,61 @@
       <c r="AK20" s="1"/>
     </row>
     <row r="21" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="21">
         <v>60.971510000000002</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="21">
         <v>138.411</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="21">
         <v>1555</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="32">
         <v>44758</v>
       </c>
-      <c r="G21" s="30" t="s">
+      <c r="G21" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H21" s="18">
+      <c r="H21" s="11">
         <v>113</v>
       </c>
-      <c r="I21" s="18">
+      <c r="I21" s="11">
         <v>210</v>
       </c>
-      <c r="J21" s="18">
+      <c r="J21" s="11">
         <v>147</v>
       </c>
-      <c r="K21" s="18">
+      <c r="K21" s="11">
         <v>94</v>
       </c>
-      <c r="L21" s="18">
+      <c r="L21" s="11">
         <v>136</v>
       </c>
-      <c r="M21" s="18">
+      <c r="M21" s="11">
         <v>95</v>
       </c>
-      <c r="N21" s="18">
+      <c r="N21" s="11">
         <v>52</v>
       </c>
-      <c r="O21" s="18">
+      <c r="O21" s="11">
         <v>56</v>
       </c>
-      <c r="P21" s="18">
+      <c r="P21" s="11">
         <v>53</v>
       </c>
-      <c r="Q21" s="18">
+      <c r="Q21" s="11">
         <v>33</v>
       </c>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="18"/>
-      <c r="U21" s="17"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="12"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
@@ -2244,58 +2242,58 @@
       <c r="A22" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="21">
         <v>60.969850000000001</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="21">
         <v>138.41273000000001</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="21">
         <v>1587</v>
       </c>
-      <c r="F22" s="30">
+      <c r="F22" s="32">
         <v>44758</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H22" s="18">
+      <c r="H22" s="11">
         <v>6.1</v>
       </c>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="18">
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="11">
         <v>16</v>
       </c>
-      <c r="L22" s="18">
+      <c r="L22" s="11">
         <v>34</v>
       </c>
-      <c r="M22" s="18">
+      <c r="M22" s="11">
         <v>27</v>
       </c>
-      <c r="N22" s="18">
+      <c r="N22" s="11">
         <v>45</v>
       </c>
-      <c r="O22" s="18">
+      <c r="O22" s="11">
         <v>27</v>
       </c>
-      <c r="P22" s="18">
+      <c r="P22" s="11">
         <v>35</v>
       </c>
-      <c r="Q22" s="18">
+      <c r="Q22" s="11">
         <v>2</v>
       </c>
-      <c r="R22" s="18">
+      <c r="R22" s="11">
         <v>3</v>
       </c>
-      <c r="S22" s="18">
+      <c r="S22" s="11">
         <v>5</v>
       </c>
-      <c r="T22" s="18"/>
-      <c r="U22" s="17"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="12"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
@@ -2317,58 +2315,58 @@
       <c r="A23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="25">
+      <c r="C23" s="21">
         <v>60.96987</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="21">
         <v>138.41272000000001</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="21">
         <v>1582</v>
       </c>
-      <c r="F23" s="30">
+      <c r="F23" s="32">
         <v>44758</v>
       </c>
-      <c r="G23" s="30" t="s">
+      <c r="G23" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H23" s="18">
+      <c r="H23" s="11">
         <v>8.5</v>
       </c>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="18">
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="11">
         <v>32</v>
       </c>
-      <c r="L23" s="18">
+      <c r="L23" s="11">
         <v>33</v>
       </c>
-      <c r="M23" s="18">
+      <c r="M23" s="11">
         <v>36</v>
       </c>
-      <c r="N23" s="18">
+      <c r="N23" s="11">
         <v>52</v>
       </c>
-      <c r="O23" s="18">
+      <c r="O23" s="11">
         <v>37</v>
       </c>
-      <c r="P23" s="18">
+      <c r="P23" s="11">
         <v>45</v>
       </c>
-      <c r="Q23" s="18">
+      <c r="Q23" s="11">
         <v>4</v>
       </c>
-      <c r="R23" s="17">
+      <c r="R23" s="12">
         <v>3</v>
       </c>
-      <c r="S23" s="17">
+      <c r="S23" s="12">
         <v>5</v>
       </c>
-      <c r="T23" s="14"/>
-      <c r="U23" s="14"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
@@ -2390,58 +2388,58 @@
       <c r="A24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="25">
+      <c r="C24" s="21">
         <v>60.969859999999997</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="21">
         <v>138.41269</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="21">
         <v>1582</v>
       </c>
-      <c r="F24" s="30">
+      <c r="F24" s="32">
         <v>44758</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="G24" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H24" s="11">
         <v>6.5</v>
       </c>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="18">
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="11">
         <v>24</v>
       </c>
-      <c r="L24" s="18">
+      <c r="L24" s="11">
         <v>36</v>
       </c>
-      <c r="M24" s="18">
+      <c r="M24" s="11">
         <v>24</v>
       </c>
-      <c r="N24" s="18">
+      <c r="N24" s="11">
         <v>35</v>
       </c>
-      <c r="O24" s="18">
+      <c r="O24" s="11">
         <v>22</v>
       </c>
-      <c r="P24" s="18">
+      <c r="P24" s="11">
         <v>25</v>
       </c>
-      <c r="Q24" s="18">
+      <c r="Q24" s="11">
         <v>5</v>
       </c>
-      <c r="R24" s="18">
+      <c r="R24" s="11">
         <v>4</v>
       </c>
-      <c r="S24" s="18">
+      <c r="S24" s="11">
         <v>2</v>
       </c>
-      <c r="T24" s="18"/>
-      <c r="U24" s="17"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="12"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
@@ -2463,58 +2461,58 @@
       <c r="A25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="25">
+      <c r="C25" s="21">
         <v>60.96987</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="21">
         <v>138.41261</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="21">
         <v>1583</v>
       </c>
-      <c r="F25" s="30">
+      <c r="F25" s="32">
         <v>44758</v>
       </c>
-      <c r="G25" s="30" t="s">
+      <c r="G25" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="11">
         <v>6.7</v>
       </c>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="18">
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="11">
         <v>35</v>
       </c>
-      <c r="L25" s="18">
+      <c r="L25" s="11">
         <v>23</v>
       </c>
-      <c r="M25" s="18">
+      <c r="M25" s="11">
         <v>35</v>
       </c>
-      <c r="N25" s="18">
+      <c r="N25" s="11">
         <v>35</v>
       </c>
-      <c r="O25" s="18">
+      <c r="O25" s="11">
         <v>36</v>
       </c>
-      <c r="P25" s="18">
+      <c r="P25" s="11">
         <v>27</v>
       </c>
-      <c r="Q25" s="18">
+      <c r="Q25" s="11">
         <v>3</v>
       </c>
-      <c r="R25" s="18">
+      <c r="R25" s="11">
         <v>4</v>
       </c>
-      <c r="S25" s="18">
+      <c r="S25" s="11">
         <v>4</v>
       </c>
-      <c r="T25" s="18"/>
-      <c r="U25" s="17"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="12"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
@@ -2536,58 +2534,58 @@
       <c r="A26" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="25">
+      <c r="C26" s="21">
         <v>60.96987</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="21">
         <v>138.41256999999999</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="21">
         <v>1582</v>
       </c>
-      <c r="F26" s="30">
+      <c r="F26" s="32">
         <v>44758</v>
       </c>
-      <c r="G26" s="30" t="s">
+      <c r="G26" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H26" s="18">
+      <c r="H26" s="11">
         <v>6.1</v>
       </c>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="18">
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="11">
         <v>40</v>
       </c>
-      <c r="L26" s="18">
+      <c r="L26" s="11">
         <v>28</v>
       </c>
-      <c r="M26" s="18">
+      <c r="M26" s="11">
         <v>36</v>
       </c>
-      <c r="N26" s="18">
+      <c r="N26" s="11">
         <v>31</v>
       </c>
-      <c r="O26" s="18">
+      <c r="O26" s="11">
         <v>21</v>
       </c>
-      <c r="P26" s="18">
+      <c r="P26" s="11">
         <v>39</v>
       </c>
-      <c r="Q26" s="18">
+      <c r="Q26" s="11">
         <v>6</v>
       </c>
-      <c r="R26" s="18">
+      <c r="R26" s="11">
         <v>5</v>
       </c>
-      <c r="S26" s="18">
+      <c r="S26" s="11">
         <v>4</v>
       </c>
-      <c r="T26" s="18"/>
-      <c r="U26" s="17"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="12"/>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
@@ -2609,58 +2607,58 @@
       <c r="A27" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="25">
+      <c r="C27" s="21">
         <v>60.97195</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="21">
         <v>138.41202999999999</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="21">
         <v>1549</v>
       </c>
-      <c r="F27" s="30">
+      <c r="F27" s="32">
         <v>44758</v>
       </c>
-      <c r="G27" s="30" t="s">
+      <c r="G27" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="18">
+      <c r="H27" s="11">
         <v>8.5</v>
       </c>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="18">
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="11">
         <v>25</v>
       </c>
-      <c r="L27" s="18">
+      <c r="L27" s="11">
         <v>30</v>
       </c>
-      <c r="M27" s="18">
+      <c r="M27" s="11">
         <v>40</v>
       </c>
-      <c r="N27" s="18">
+      <c r="N27" s="11">
         <v>31</v>
       </c>
-      <c r="O27" s="18">
+      <c r="O27" s="11">
         <v>49</v>
       </c>
-      <c r="P27" s="18">
+      <c r="P27" s="11">
         <v>45</v>
       </c>
-      <c r="Q27" s="18">
+      <c r="Q27" s="11">
         <v>3</v>
       </c>
-      <c r="R27" s="18">
+      <c r="R27" s="11">
         <v>4</v>
       </c>
-      <c r="S27" s="18">
+      <c r="S27" s="11">
         <v>3</v>
       </c>
-      <c r="T27" s="18"/>
-      <c r="U27" s="17"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="12"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
@@ -2682,58 +2680,58 @@
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="25">
+      <c r="C28" s="21">
         <v>60.971960000000003</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="21">
         <v>138.41202999999999</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="21">
         <v>1548</v>
       </c>
-      <c r="F28" s="30">
+      <c r="F28" s="32">
         <v>44758</v>
       </c>
-      <c r="G28" s="30" t="s">
+      <c r="G28" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H28" s="22">
         <v>5.6</v>
       </c>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="18">
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="11">
         <v>28</v>
       </c>
-      <c r="L28" s="18">
+      <c r="L28" s="11">
         <v>20</v>
       </c>
-      <c r="M28" s="18">
+      <c r="M28" s="11">
         <v>25</v>
       </c>
-      <c r="N28" s="18">
+      <c r="N28" s="11">
         <v>29</v>
       </c>
-      <c r="O28" s="18">
+      <c r="O28" s="11">
         <v>38</v>
       </c>
-      <c r="P28" s="18">
+      <c r="P28" s="11">
         <v>42</v>
       </c>
-      <c r="Q28" s="18">
+      <c r="Q28" s="11">
         <v>3</v>
       </c>
-      <c r="R28" s="18">
+      <c r="R28" s="11">
         <v>3</v>
       </c>
-      <c r="S28" s="18">
+      <c r="S28" s="11">
         <v>2</v>
       </c>
-      <c r="T28" s="19"/>
-      <c r="U28" s="14"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="13"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
@@ -2755,58 +2753,58 @@
       <c r="A29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="25">
+      <c r="C29" s="21">
         <v>60.97195</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="21">
         <v>138.41206</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="21">
         <v>1549</v>
       </c>
-      <c r="F29" s="30">
+      <c r="F29" s="32">
         <v>44758</v>
       </c>
-      <c r="G29" s="30" t="s">
+      <c r="G29" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H29" s="26">
+      <c r="H29" s="22">
         <v>4.5</v>
       </c>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="26">
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="22">
         <v>20</v>
       </c>
-      <c r="L29" s="26">
+      <c r="L29" s="22">
         <v>10</v>
       </c>
-      <c r="M29" s="26">
+      <c r="M29" s="22">
         <v>28</v>
       </c>
-      <c r="N29" s="26">
+      <c r="N29" s="22">
         <v>26</v>
       </c>
-      <c r="O29" s="26">
+      <c r="O29" s="22">
         <v>31</v>
       </c>
-      <c r="P29" s="26">
+      <c r="P29" s="22">
         <v>34</v>
       </c>
-      <c r="Q29" s="26">
+      <c r="Q29" s="22">
         <v>4</v>
       </c>
-      <c r="R29" s="26">
+      <c r="R29" s="22">
         <v>3</v>
       </c>
-      <c r="S29" s="26">
+      <c r="S29" s="22">
         <v>4</v>
       </c>
-      <c r="T29" s="19"/>
-      <c r="U29" s="14"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="13"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
@@ -2828,58 +2826,58 @@
       <c r="A30" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="25">
+      <c r="C30" s="21">
         <v>60.971499999999999</v>
       </c>
-      <c r="D30" s="25">
+      <c r="D30" s="21">
         <v>138.41105999999999</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="21">
         <v>1554</v>
       </c>
-      <c r="F30" s="30">
+      <c r="F30" s="32">
         <v>44758</v>
       </c>
-      <c r="G30" s="30" t="s">
+      <c r="G30" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H30" s="26">
+      <c r="H30" s="22">
         <v>8.5</v>
       </c>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="26">
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="22">
         <v>35</v>
       </c>
-      <c r="L30" s="26">
+      <c r="L30" s="22">
         <v>18</v>
       </c>
-      <c r="M30" s="26">
+      <c r="M30" s="22">
         <v>24</v>
       </c>
-      <c r="N30" s="26">
+      <c r="N30" s="22">
         <v>38</v>
       </c>
-      <c r="O30" s="26">
+      <c r="O30" s="22">
         <v>28</v>
       </c>
-      <c r="P30" s="26">
+      <c r="P30" s="22">
         <v>25</v>
       </c>
-      <c r="Q30" s="26">
+      <c r="Q30" s="22">
         <v>4</v>
       </c>
-      <c r="R30" s="26">
+      <c r="R30" s="22">
         <v>3</v>
       </c>
-      <c r="S30" s="26">
+      <c r="S30" s="22">
         <v>2</v>
       </c>
-      <c r="T30" s="19"/>
-      <c r="U30" s="14"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="13"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
@@ -2901,58 +2899,58 @@
       <c r="A31" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="25">
+      <c r="C31" s="21">
         <v>60.971519999999998</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="21">
         <v>138.41103000000001</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="21">
         <v>1555</v>
       </c>
-      <c r="F31" s="30">
+      <c r="F31" s="32">
         <v>44758</v>
       </c>
-      <c r="G31" s="30" t="s">
+      <c r="G31" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H31" s="26">
+      <c r="H31" s="22">
         <v>8.5</v>
       </c>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="26">
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="22">
         <v>12</v>
       </c>
-      <c r="L31" s="26">
+      <c r="L31" s="22">
         <v>17</v>
       </c>
-      <c r="M31" s="26">
+      <c r="M31" s="22">
         <v>22</v>
       </c>
-      <c r="N31" s="26">
+      <c r="N31" s="22">
         <v>44</v>
       </c>
-      <c r="O31" s="26">
+      <c r="O31" s="22">
         <v>39</v>
       </c>
-      <c r="P31" s="26">
+      <c r="P31" s="22">
         <v>25</v>
       </c>
-      <c r="Q31" s="26">
+      <c r="Q31" s="22">
         <v>3</v>
       </c>
-      <c r="R31" s="26">
+      <c r="R31" s="22">
         <v>3</v>
       </c>
-      <c r="S31" s="26">
+      <c r="S31" s="22">
         <v>4</v>
       </c>
-      <c r="T31" s="19"/>
-      <c r="U31" s="14"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="13"/>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
@@ -2972,26 +2970,26 @@
     </row>
     <row r="32" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="22"/>
-      <c r="S32" s="22"/>
-      <c r="T32" s="19"/>
-      <c r="U32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="13"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
@@ -3011,26 +3009,26 @@
     </row>
     <row r="33" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
-      <c r="Q33" s="22"/>
-      <c r="R33" s="22"/>
-      <c r="S33" s="22"/>
-      <c r="T33" s="19"/>
-      <c r="U33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="13"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
@@ -3050,26 +3048,26 @@
     </row>
     <row r="34" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="22"/>
-      <c r="S34" s="22"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="13"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
@@ -3089,26 +3087,26 @@
     </row>
     <row r="35" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
-      <c r="Q35" s="22"/>
-      <c r="R35" s="22"/>
-      <c r="S35" s="22"/>
-      <c r="T35" s="19"/>
-      <c r="U35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="13"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
@@ -3128,26 +3126,26 @@
     </row>
     <row r="36" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="22"/>
-      <c r="Q36" s="22"/>
-      <c r="R36" s="22"/>
-      <c r="S36" s="22"/>
-      <c r="T36" s="19"/>
-      <c r="U36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
+      <c r="T36" s="10"/>
+      <c r="U36" s="13"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
@@ -3167,26 +3165,26 @@
     </row>
     <row r="37" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
-      <c r="T37" s="15"/>
-      <c r="U37" s="23"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="19"/>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
@@ -3206,26 +3204,26 @@
     </row>
     <row r="38" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
-      <c r="T38" s="19"/>
-      <c r="U38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="13"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
@@ -3245,26 +3243,26 @@
     </row>
     <row r="39" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="19"/>
-      <c r="U39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="13"/>
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
@@ -3284,26 +3282,26 @@
     </row>
     <row r="40" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="15"/>
-      <c r="U40" s="23"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="19"/>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
@@ -3323,26 +3321,26 @@
     </row>
     <row r="41" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
-      <c r="T41" s="22"/>
-      <c r="U41" s="24"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
+      <c r="T41" s="18"/>
+      <c r="U41" s="20"/>
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
@@ -3362,26 +3360,26 @@
     </row>
     <row r="42" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="19"/>
-      <c r="U42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="13"/>
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
@@ -3401,26 +3399,26 @@
     </row>
     <row r="43" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="25"/>
-      <c r="O43" s="25"/>
-      <c r="P43" s="25"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="T43" s="19"/>
-      <c r="U43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="21"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="13"/>
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
@@ -3440,26 +3438,26 @@
     </row>
     <row r="44" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="25"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="19"/>
-      <c r="U44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="21"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="10"/>
+      <c r="U44" s="13"/>
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
@@ -3479,26 +3477,26 @@
     </row>
     <row r="45" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="25"/>
-      <c r="P45" s="25"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
-      <c r="T45" s="19"/>
-      <c r="U45" s="14"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="21"/>
+      <c r="P45" s="21"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="10"/>
+      <c r="U45" s="13"/>
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
@@ -3518,26 +3516,26 @@
     </row>
     <row r="46" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
-      <c r="T46" s="19"/>
-      <c r="U46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="10"/>
+      <c r="U46" s="13"/>
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
@@ -3557,26 +3555,26 @@
     </row>
     <row r="47" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="19"/>
-      <c r="U47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="10"/>
+      <c r="U47" s="13"/>
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
@@ -3596,26 +3594,26 @@
     </row>
     <row r="48" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="18"/>
-      <c r="O48" s="18"/>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="18"/>
-      <c r="T48" s="19"/>
-      <c r="U48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="10"/>
+      <c r="U48" s="13"/>
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
@@ -3635,26 +3633,26 @@
     </row>
     <row r="49" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
-      <c r="L49" s="18"/>
-      <c r="M49" s="18"/>
-      <c r="N49" s="18"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="18"/>
-      <c r="Q49" s="18"/>
-      <c r="R49" s="18"/>
-      <c r="S49" s="18"/>
-      <c r="T49" s="19"/>
-      <c r="U49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
+      <c r="R49" s="11"/>
+      <c r="S49" s="11"/>
+      <c r="T49" s="10"/>
+      <c r="U49" s="13"/>
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
@@ -3674,26 +3672,26 @@
     </row>
     <row r="50" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="22"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="22"/>
-      <c r="O50" s="22"/>
-      <c r="P50" s="22"/>
-      <c r="Q50" s="22"/>
-      <c r="R50" s="22"/>
-      <c r="S50" s="22"/>
-      <c r="T50" s="19"/>
-      <c r="U50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="18"/>
+      <c r="Q50" s="18"/>
+      <c r="R50" s="18"/>
+      <c r="S50" s="18"/>
+      <c r="T50" s="10"/>
+      <c r="U50" s="13"/>
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
@@ -3713,26 +3711,26 @@
     </row>
     <row r="51" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="22"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="22"/>
-      <c r="M51" s="22"/>
-      <c r="N51" s="22"/>
-      <c r="O51" s="22"/>
-      <c r="P51" s="22"/>
-      <c r="Q51" s="22"/>
-      <c r="R51" s="22"/>
-      <c r="S51" s="22"/>
-      <c r="T51" s="19"/>
-      <c r="U51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="18"/>
+      <c r="O51" s="18"/>
+      <c r="P51" s="18"/>
+      <c r="Q51" s="18"/>
+      <c r="R51" s="18"/>
+      <c r="S51" s="18"/>
+      <c r="T51" s="10"/>
+      <c r="U51" s="13"/>
       <c r="V51" s="1"/>
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
@@ -3752,26 +3750,26 @@
     </row>
     <row r="52" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="22"/>
-      <c r="J52" s="22"/>
-      <c r="K52" s="22"/>
-      <c r="L52" s="22"/>
-      <c r="M52" s="22"/>
-      <c r="N52" s="22"/>
-      <c r="O52" s="22"/>
-      <c r="P52" s="22"/>
-      <c r="Q52" s="22"/>
-      <c r="R52" s="22"/>
-      <c r="S52" s="22"/>
-      <c r="T52" s="19"/>
-      <c r="U52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="18"/>
+      <c r="P52" s="18"/>
+      <c r="Q52" s="18"/>
+      <c r="R52" s="18"/>
+      <c r="S52" s="18"/>
+      <c r="T52" s="10"/>
+      <c r="U52" s="13"/>
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
       <c r="X52" s="1"/>
@@ -3791,26 +3789,26 @@
     </row>
     <row r="53" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="22"/>
-      <c r="I53" s="22"/>
-      <c r="J53" s="22"/>
-      <c r="K53" s="22"/>
-      <c r="L53" s="22"/>
-      <c r="M53" s="22"/>
-      <c r="N53" s="22"/>
-      <c r="O53" s="22"/>
-      <c r="P53" s="22"/>
-      <c r="Q53" s="22"/>
-      <c r="R53" s="22"/>
-      <c r="S53" s="22"/>
-      <c r="T53" s="19"/>
-      <c r="U53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+      <c r="P53" s="18"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18"/>
+      <c r="S53" s="18"/>
+      <c r="T53" s="10"/>
+      <c r="U53" s="13"/>
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
@@ -3830,26 +3828,26 @@
     </row>
     <row r="54" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="22"/>
-      <c r="I54" s="22"/>
-      <c r="J54" s="22"/>
-      <c r="K54" s="22"/>
-      <c r="L54" s="22"/>
-      <c r="M54" s="22"/>
-      <c r="N54" s="22"/>
-      <c r="O54" s="22"/>
-      <c r="P54" s="22"/>
-      <c r="Q54" s="22"/>
-      <c r="R54" s="22"/>
-      <c r="S54" s="22"/>
-      <c r="T54" s="19"/>
-      <c r="U54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+      <c r="N54" s="18"/>
+      <c r="O54" s="18"/>
+      <c r="P54" s="18"/>
+      <c r="Q54" s="18"/>
+      <c r="R54" s="18"/>
+      <c r="S54" s="18"/>
+      <c r="T54" s="10"/>
+      <c r="U54" s="13"/>
       <c r="V54" s="1"/>
       <c r="W54" s="1"/>
       <c r="X54" s="1"/>
@@ -3869,26 +3867,26 @@
     </row>
     <row r="55" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="22"/>
-      <c r="I55" s="22"/>
-      <c r="J55" s="22"/>
-      <c r="K55" s="22"/>
-      <c r="L55" s="22"/>
-      <c r="M55" s="22"/>
-      <c r="N55" s="22"/>
-      <c r="O55" s="22"/>
-      <c r="P55" s="22"/>
-      <c r="Q55" s="22"/>
-      <c r="R55" s="22"/>
-      <c r="S55" s="22"/>
-      <c r="T55" s="19"/>
-      <c r="U55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="18"/>
+      <c r="N55" s="18"/>
+      <c r="O55" s="18"/>
+      <c r="P55" s="18"/>
+      <c r="Q55" s="18"/>
+      <c r="R55" s="18"/>
+      <c r="S55" s="18"/>
+      <c r="T55" s="10"/>
+      <c r="U55" s="13"/>
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
       <c r="X55" s="1"/>

</xml_diff>